<commit_message>
updated with title, and refactoring
</commit_message>
<xml_diff>
--- a/bingo_bango.xlsx
+++ b/bingo_bango.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\musikbingo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\musik1\Music_bingo_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{261877FD-9D9B-481F-80C7-02992EF0FCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5739A306-59AD-427F-88A5-38F708F56EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{9D8F021D-FE5D-4449-821D-D70C4531D842}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{9D8F021D-FE5D-4449-821D-D70C4531D842}"/>
   </bookViews>
   <sheets>
     <sheet name="bingo_plates" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Bingo Plate Number</t>
   </si>
@@ -31,129 +44,6 @@
     <t>Last 5 Numbers</t>
   </si>
   <si>
-    <t>0. Baby One More Time - Britney Spears - 1998</t>
-  </si>
-  <si>
-    <t>1. I Want It That Way - Backstreet Boys - 1999</t>
-  </si>
-  <si>
-    <t>2. Genie in a Bottle - Christina Aguilera - 1999</t>
-  </si>
-  <si>
-    <t>3. Livin' la Vida Loca - Ricky Martin - 1999</t>
-  </si>
-  <si>
-    <t>4. Wannabe - Spice Girls - 1996</t>
-  </si>
-  <si>
-    <t>5. Torn - Natalie Imbruglia - 1997</t>
-  </si>
-  <si>
-    <t>6. No Scrubs - TLC - 1999</t>
-  </si>
-  <si>
-    <t>7. Believe - Cher - 1998</t>
-  </si>
-  <si>
-    <t>8. Smooth - Santana ft. Rob Thomas - 1999</t>
-  </si>
-  <si>
-    <t>9. I Will Always Love You - Whitney Houston - 1992</t>
-  </si>
-  <si>
-    <t>10. My Heart Will Go On - Celine Dion - 1997</t>
-  </si>
-  <si>
-    <t>11. I Want You Back - *NSYNC - 1996</t>
-  </si>
-  <si>
-    <t>12. Waterfalls - TLC - 1994</t>
-  </si>
-  <si>
-    <t>13. Bitter Sweet Symphony - The Verve - 1997</t>
-  </si>
-  <si>
-    <t>14. Iris - Goo Goo Dolls - 1998</t>
-  </si>
-  <si>
-    <t>15. Say My Name - Destiny's Child - 1999</t>
-  </si>
-  <si>
-    <t>16. Kiss Me - Sixpence None The Richer - 1997</t>
-  </si>
-  <si>
-    <t>17. Un-Break My Heart - Toni Braxton - 1996</t>
-  </si>
-  <si>
-    <t>18. Truly Madly Deeply - Savage Garden - 1997</t>
-  </si>
-  <si>
-    <t>19. I'll Be Missing You - Puff Daddy ft. Faith Evans - 1997</t>
-  </si>
-  <si>
-    <t>20. Don't Speak - No Doubt - 1995</t>
-  </si>
-  <si>
-    <t>21. All Star - Smash Mouth - 1999</t>
-  </si>
-  <si>
-    <t>22. I Want You - Savage Garden - 1996</t>
-  </si>
-  <si>
-    <t>23. Tearin' Up My Heart - *NSYNC - 1997</t>
-  </si>
-  <si>
-    <t>24. I Don't Want to Miss a Thing - Aerosmith - 1998</t>
-  </si>
-  <si>
-    <t>25. The Boy Is Mine - Brandy &amp; Monica - 1998</t>
-  </si>
-  <si>
-    <t>26. Bailamos - Enrique Iglesias - 1999</t>
-  </si>
-  <si>
-    <t>27. I Want You Back - Savage Garden - 1996</t>
-  </si>
-  <si>
-    <t>28. You're Still the One - Shania Twain - 1997</t>
-  </si>
-  <si>
-    <t>29. I'll Be There for You - The Rembrandts - 1995</t>
-  </si>
-  <si>
-    <t>30. Smooth Criminal - Alien Ant Farm - 2001</t>
-  </si>
-  <si>
-    <t>31. Mambo No. 5 (A Little Bit of...) - Lou Bega - 1999</t>
-  </si>
-  <si>
-    <t>32. I Want You to Want Me - Letters to Cleo - 1999</t>
-  </si>
-  <si>
-    <t>33. Iris - Goo Goo Dolls - 1998</t>
-  </si>
-  <si>
-    <t>34. Bailamos - Enrique Iglesias - 1999</t>
-  </si>
-  <si>
-    <t>35. I Want You Back - *NSYNC - 1996</t>
-  </si>
-  <si>
-    <t>36. No Rain - Blind Melon - 1992</t>
-  </si>
-  <si>
-    <t>37. I Will Always Love You - Whitney Houston - 1992</t>
-  </si>
-  <si>
-    <t>38. My Own Worst Enemy - Lit - 1999</t>
-  </si>
-  <si>
-    <t>39. I Want It That Way - Backstreet Boys - 1999</t>
-  </si>
-  <si>
-    <t>40. Genie in a Bottle - Christina Aguilera - 1999</t>
-  </si>
-  <si>
     <t>Katalog</t>
   </si>
   <si>
@@ -164,6 +54,108 @@
   </si>
   <si>
     <t>Række 2</t>
+  </si>
+  <si>
+    <t>0. Smuk som et stjerneskud - Brødrene Olsen - 1990</t>
+  </si>
+  <si>
+    <t>1. Mamma Mia - ABB - 1975</t>
+  </si>
+  <si>
+    <t>2. Jalousi - Medina - 2009</t>
+  </si>
+  <si>
+    <t>3. Girls Just Want to Have Fun - Cyndi Lauper - 1983</t>
+  </si>
+  <si>
+    <t>4. I Will Survive - Gloria Gaynor - 1978</t>
+  </si>
+  <si>
+    <t>5. Kongen Af Danmark - Malte Ebert - 1999</t>
+  </si>
+  <si>
+    <t>6. Kom Tilbage Nu - Danseorkestret - 1985</t>
+  </si>
+  <si>
+    <t>7. Jeg Vil La`Lyset brænde - Ray Dee Ohh - 1988</t>
+  </si>
+  <si>
+    <t>8. Sig Du Ka´Li´Mig - Tøsedrengene - 1985</t>
+  </si>
+  <si>
+    <t>9. Hold Me Now - Johnny Logan - 1987</t>
+  </si>
+  <si>
+    <t>10. Only Teardrops - Emmelie de Forest - 2013</t>
+  </si>
+  <si>
+    <t>11. I En Lille Båd Der Gynger - Bamses Venner - 1980</t>
+  </si>
+  <si>
+    <t>12. I Want It That Way - Backstreet Boys - 1999</t>
+  </si>
+  <si>
+    <t>13. Billie Jean - Michael Jackson - 1982</t>
+  </si>
+  <si>
+    <t>14. Øde Ø - Rasmus Seebach - 2011</t>
+  </si>
+  <si>
+    <t>15. Believe - Cher - 1998</t>
+  </si>
+  <si>
+    <t>16. Kiss - Prince - 1986</t>
+  </si>
+  <si>
+    <t>17. Vågner I natten - Dodo &amp; the Dodos - 1987</t>
+  </si>
+  <si>
+    <t>18. Stayin´Alive - Bee Gees - 1977</t>
+  </si>
+  <si>
+    <t>19. De Første Kærester På Månen - TV-2 - 1986</t>
+  </si>
+  <si>
+    <t>20. Hvor ska´vi sove i nat - Laban - 1982</t>
+  </si>
+  <si>
+    <t>21. Bohemian Rhapsody - Queen - 1975</t>
+  </si>
+  <si>
+    <t>22. Don´t Go Breaking My Heart - Elton John</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kiki Dee - 1976</t>
+  </si>
+  <si>
+    <t>23. Oh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pretty Woman - Roy Orbison - 1964</t>
+  </si>
+  <si>
+    <t>24. Imagine - John Lennon - 1971</t>
+  </si>
+  <si>
+    <t>25. Kender du det? - Søren Kragh-Jacobsen - 1985</t>
+  </si>
+  <si>
+    <t>26. En som dig - Back To Back - 1989</t>
+  </si>
+  <si>
+    <t>27. STOR MAND - Tobias Rahim</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Andreas Odbjerg - 2020</t>
+  </si>
+  <si>
+    <t>28. I will Always Love You - Whitney Houston - 1992</t>
+  </si>
+  <si>
+    <t>29. Glor På Vinduer - Anne Linnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marquis De Sade - 1986</t>
   </si>
 </sst>
 </file>
@@ -659,57 +651,56 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Farve1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Farve2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Farve3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Farve4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Farve5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Farve6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Farve1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Farve2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Farve3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Farve4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Farve5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Farve6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Farve1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Farve2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Farve3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Farve4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Farve5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Farve6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Advarselstekst" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Bemærk!" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Beregning" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Farve1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Farve2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Farve3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Farve4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Farve5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Farve6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Forklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="God" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Kontrollér celle" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Overskrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Overskrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Overskrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Overskrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Sammenkædet celle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Ugyldig" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,7 +716,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1041,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E017F0-A62F-4B1C-A88C-D0953833BE1E}">
-  <dimension ref="A1:S42"/>
+  <dimension ref="A1:Z31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33:V42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1055,8 +1046,8 @@
     <col min="18" max="18" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1066,59 +1057,59 @@
         <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="S1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>17</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
       <c r="I2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M2">
         <f>COUNTIF($Q$2:$Q$29,B2)+COUNTIF($Q$2:$Q$29,C2)+COUNTIF($Q$2:$Q$29,D2)+COUNTIF($Q$2:$Q$29,E2)+COUNTIF($Q$2:$Q$29,F2)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N2">
         <f>COUNTIF($Q$2:$Q$29,G2)+COUNTIF($Q$2:$Q$29,H2)+COUNTIF($Q$2:$Q$29,I2)+COUNTIF($Q$2:$Q$29,J2)+COUNTIF($Q$2:$Q$29,K2)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O2" t="str">
         <f>IF(M2=5,"Bango","")</f>
@@ -1128,52 +1119,54 @@
         <f>IF(N2=5,"Bango","")</f>
         <v/>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
       <c r="S2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>24</v>
       </c>
       <c r="G3">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H3">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="I3">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="J3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M29" si="0">COUNTIF($Q$2:$Q$29,B3)+COUNTIF($Q$2:$Q$29,C3)+COUNTIF($Q$2:$Q$29,D3)+COUNTIF($Q$2:$Q$29,E3)+COUNTIF($Q$2:$Q$29,F3)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N29" si="1">COUNTIF($Q$2:$Q$29,G3)+COUNTIF($Q$2:$Q$29,H3)+COUNTIF($Q$2:$Q$29,I3)+COUNTIF($Q$2:$Q$29,J3)+COUNTIF($Q$2:$Q$29,K3)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O29" si="2">IF(M3=5,"Bango","")</f>
@@ -1183,52 +1176,54 @@
         <f t="shared" ref="P3:P29" si="3">IF(N3=5,"Bango","")</f>
         <v/>
       </c>
-      <c r="Q3" s="1"/>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
       <c r="S3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A4" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
         <v>13</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>9</v>
-      </c>
-      <c r="J4">
-        <v>23</v>
-      </c>
-      <c r="K4">
-        <v>28</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="2"/>
@@ -1236,219 +1231,227 @@
       </c>
       <c r="P4" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="Q4" s="1"/>
+        <v>Bango</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2</v>
+      </c>
       <c r="S4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A5" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5">
+        <v>21</v>
+      </c>
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
       <c r="D5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>24</v>
+      </c>
+      <c r="K5">
         <v>14</v>
-      </c>
-      <c r="G5">
-        <v>19</v>
-      </c>
-      <c r="H5">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>11</v>
-      </c>
-      <c r="K5">
-        <v>25</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Bango</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1">
+        <v>3</v>
+      </c>
       <c r="S5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C6">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
         <v>18</v>
       </c>
-      <c r="D6">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>22</v>
-      </c>
       <c r="F6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="K6">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Bango</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="Q6" s="1"/>
+        <v>Bango</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>4</v>
+      </c>
       <c r="S6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7">
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>20</v>
+      </c>
+      <c r="J7">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>17</v>
-      </c>
-      <c r="D7">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>15</v>
-      </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7">
+      <c r="K7">
         <v>25</v>
-      </c>
-      <c r="H7">
-        <v>30</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>19</v>
-      </c>
-      <c r="K7">
-        <v>21</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Bango</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q7" s="1"/>
+      <c r="Q7" s="1">
+        <v>5</v>
+      </c>
       <c r="S7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A8" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8">
+        <v>13</v>
+      </c>
+      <c r="I8">
+        <v>14</v>
+      </c>
+      <c r="J8">
         <v>27</v>
       </c>
-      <c r="I8">
-        <v>28</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
-      </c>
       <c r="K8">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="2"/>
@@ -1458,52 +1461,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q8" s="1"/>
+      <c r="Q8" s="1">
+        <v>6</v>
+      </c>
       <c r="S8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A9" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I9">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="J9">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="2"/>
@@ -1511,54 +1516,56 @@
       </c>
       <c r="P9" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="Q9" s="1"/>
+        <v>Bango</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>7</v>
+      </c>
       <c r="S9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A10" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <v>14</v>
+      </c>
+      <c r="J10">
         <v>7</v>
       </c>
-      <c r="E10">
-        <v>16</v>
-      </c>
-      <c r="F10">
-        <v>29</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>22</v>
-      </c>
-      <c r="I10">
-        <v>17</v>
-      </c>
-      <c r="J10">
-        <v>8</v>
-      </c>
       <c r="K10">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="2"/>
@@ -1568,52 +1575,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q10" s="1"/>
+      <c r="Q10" s="1">
+        <v>8</v>
+      </c>
       <c r="S10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11">
+      <c r="D11">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>27</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>14</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
       <c r="J11">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="K11">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="2"/>
@@ -1623,52 +1632,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="1">
+        <v>9</v>
+      </c>
       <c r="S11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E12">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="I12">
+        <v>26</v>
+      </c>
+      <c r="J12">
         <v>28</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1</v>
-      </c>
-      <c r="K12">
-        <v>13</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" si="2"/>
@@ -1678,52 +1689,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="1">
+        <v>10</v>
+      </c>
       <c r="S12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G13">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H13">
         <v>11</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="J13">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="K13">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="2"/>
@@ -1733,52 +1746,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q13" s="1"/>
+      <c r="Q13" s="1">
+        <v>15</v>
+      </c>
       <c r="S13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A14" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>23</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
         <v>17</v>
       </c>
-      <c r="F14">
-        <v>22</v>
-      </c>
-      <c r="G14">
-        <v>21</v>
-      </c>
-      <c r="H14">
-        <v>28</v>
-      </c>
-      <c r="I14">
-        <v>13</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
       <c r="K14">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="2"/>
@@ -1788,52 +1803,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q14" s="1"/>
+      <c r="Q14" s="1">
+        <v>16</v>
+      </c>
       <c r="S14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A15" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E15">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F15">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I15">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="J15">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K15">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="2"/>
@@ -1843,52 +1860,60 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q15" s="1"/>
+      <c r="Q15" s="1">
+        <v>11</v>
+      </c>
       <c r="S15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+        <v>20</v>
+      </c>
+      <c r="Y15">
+        <v>4</v>
+      </c>
+      <c r="Z15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D16">
         <v>27</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>24</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>26</v>
+      </c>
+      <c r="K16">
         <v>2</v>
-      </c>
-      <c r="H16">
-        <v>9</v>
-      </c>
-      <c r="I16">
-        <v>26</v>
-      </c>
-      <c r="J16">
-        <v>29</v>
-      </c>
-      <c r="K16">
-        <v>24</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" si="2"/>
@@ -1898,52 +1923,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q16" s="1"/>
+      <c r="Q16" s="1">
+        <v>12</v>
+      </c>
       <c r="S16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A17" s="2">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>25</v>
+      </c>
+      <c r="F17">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17">
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>21</v>
+      </c>
+      <c r="I17">
+        <v>18</v>
+      </c>
+      <c r="J17">
+        <v>11</v>
+      </c>
+      <c r="K17">
         <v>14</v>
-      </c>
-      <c r="C17">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>15</v>
-      </c>
-      <c r="E17">
-        <v>21</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>19</v>
-      </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-      <c r="I17">
-        <v>30</v>
-      </c>
-      <c r="J17">
-        <v>20</v>
-      </c>
-      <c r="K17">
-        <v>18</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="2"/>
@@ -1951,54 +1978,56 @@
       </c>
       <c r="P17" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="Q17" s="1"/>
+        <v>Bango</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>13</v>
+      </c>
       <c r="S17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C18">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D18">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H18">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I18">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J18">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="K18">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="2"/>
@@ -2008,52 +2037,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q18" s="1"/>
+      <c r="Q18" s="1">
+        <v>14</v>
+      </c>
       <c r="S18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A19" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>19</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="F19">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H19">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I19">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J19">
         <v>10</v>
       </c>
       <c r="K19">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" si="2"/>
@@ -2063,52 +2094,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q19" s="1"/>
+      <c r="Q19" s="1">
+        <v>17</v>
+      </c>
       <c r="S19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A20" s="2">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>26</v>
+      </c>
+      <c r="D20">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A20" s="3">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>11</v>
-      </c>
-      <c r="C20">
-        <v>24</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
       <c r="E20">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="F20">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G20">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="H20">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="I20">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J20">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="K20">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="2"/>
@@ -2118,52 +2151,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q20" s="1"/>
+      <c r="Q20" s="1">
+        <v>18</v>
+      </c>
       <c r="S20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A21" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E21">
         <v>16</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="I21">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
         <v>26</v>
-      </c>
-      <c r="K21">
-        <v>23</v>
       </c>
       <c r="M21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="2"/>
@@ -2173,52 +2208,54 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="Q21" s="1"/>
+      <c r="Q21" s="1">
+        <v>21</v>
+      </c>
       <c r="S21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A22" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>13</v>
+      </c>
+      <c r="E22">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
         <v>8</v>
       </c>
-      <c r="D22">
+      <c r="J22">
         <v>10</v>
       </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-      <c r="F22">
-        <v>24</v>
-      </c>
-      <c r="G22">
-        <v>29</v>
-      </c>
-      <c r="H22">
-        <v>7</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>14</v>
-      </c>
       <c r="K22">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="M22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="2"/>
@@ -2226,54 +2263,54 @@
       </c>
       <c r="P22" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Bango</v>
       </c>
       <c r="Q22" s="1"/>
       <c r="S22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A23" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>13</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>25</v>
+      </c>
+      <c r="K23">
         <v>7</v>
-      </c>
-      <c r="C23">
-        <v>23</v>
-      </c>
-      <c r="D23">
-        <v>27</v>
-      </c>
-      <c r="E23">
-        <v>8</v>
-      </c>
-      <c r="F23">
-        <v>10</v>
-      </c>
-      <c r="G23">
-        <v>26</v>
-      </c>
-      <c r="H23">
-        <v>3</v>
-      </c>
-      <c r="I23">
-        <v>24</v>
-      </c>
-      <c r="J23">
-        <v>11</v>
-      </c>
-      <c r="K23">
-        <v>9</v>
       </c>
       <c r="M23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N23">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="2"/>
@@ -2285,50 +2322,50 @@
       </c>
       <c r="Q23" s="1"/>
       <c r="S23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A24" s="2">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>26</v>
+      </c>
+      <c r="F24">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A24" s="3">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>9</v>
-      </c>
-      <c r="C24">
-        <v>19</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24">
-        <v>10</v>
-      </c>
-      <c r="F24">
+      <c r="G24">
         <v>1</v>
       </c>
-      <c r="G24">
-        <v>8</v>
-      </c>
       <c r="H24">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
         <v>7</v>
       </c>
-      <c r="J24">
-        <v>22</v>
-      </c>
       <c r="K24">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="M24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="2"/>
@@ -2336,54 +2373,57 @@
       </c>
       <c r="P24" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Bango</v>
       </c>
       <c r="Q24" s="1"/>
       <c r="S24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A25" s="3">
+        <v>29</v>
+      </c>
+      <c r="T24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
         <v>18</v>
-      </c>
-      <c r="D25">
-        <v>12</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
       </c>
       <c r="F25">
         <v>22</v>
       </c>
       <c r="G25">
+        <v>26</v>
+      </c>
+      <c r="H25">
+        <v>25</v>
+      </c>
+      <c r="I25">
         <v>2</v>
       </c>
-      <c r="H25">
+      <c r="J25">
+        <v>11</v>
+      </c>
+      <c r="K25">
         <v>9</v>
-      </c>
-      <c r="I25">
-        <v>8</v>
-      </c>
-      <c r="J25">
-        <v>20</v>
-      </c>
-      <c r="K25">
-        <v>11</v>
       </c>
       <c r="M25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N25">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="2"/>
@@ -2395,50 +2435,53 @@
       </c>
       <c r="Q25" s="1"/>
       <c r="S25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A26" s="3">
+        <v>31</v>
+      </c>
+      <c r="T25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>19</v>
       </c>
-      <c r="F26">
-        <v>14</v>
-      </c>
       <c r="G26">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H26">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="I26">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="K26">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="2"/>
@@ -2450,50 +2493,50 @@
       </c>
       <c r="Q26" s="1"/>
       <c r="S26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A27" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D27">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F27">
         <v>19</v>
       </c>
       <c r="G27">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H27">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="J27">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="K27">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="M27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="2"/>
@@ -2505,50 +2548,50 @@
       </c>
       <c r="Q27" s="1"/>
       <c r="S27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A28" s="3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E28">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F28">
+        <v>16</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>18</v>
+      </c>
+      <c r="I28">
         <v>28</v>
       </c>
-      <c r="G28">
-        <v>11</v>
-      </c>
-      <c r="H28">
-        <v>26</v>
-      </c>
-      <c r="I28">
-        <v>10</v>
-      </c>
       <c r="J28">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="K28">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="M28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="2"/>
@@ -2560,50 +2603,50 @@
       </c>
       <c r="Q28" s="1"/>
       <c r="S28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A29" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E29">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H29">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="I29">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J29">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K29">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="M29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N29">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="2"/>
@@ -2615,85 +2658,23 @@
       </c>
       <c r="Q29" s="1"/>
       <c r="S29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="Q30" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="T29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
       <c r="S30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="Q31" s="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
       <c r="S31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="Q32" s="2"/>
-      <c r="S32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q33" s="2"/>
-      <c r="S33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q34" s="2"/>
-      <c r="S34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q35" s="2"/>
-      <c r="S35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q36" s="2"/>
-      <c r="S36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q37" s="2"/>
-      <c r="S37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q38" s="2"/>
-      <c r="S38" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="39" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q39" s="2"/>
-      <c r="S39" t="s">
+      <c r="T31" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q40" s="2"/>
-      <c r="S40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q41" s="2"/>
-      <c r="S41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="17:19" x14ac:dyDescent="0.45">
-      <c r="Q42" s="2"/>
-      <c r="S42" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>